<commit_message>
Added Flow till Action Center
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\B&amp;W\Updated Docs\New_BW_QAB_Performer_V1-20230215T050827Z-001\BW_QAB_Performer_V1\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ReQuoteProcess\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -231,6 +231,12 @@
   </si>
   <si>
     <t>AgentID</t>
+  </si>
+  <si>
+    <t>ClassifierConfidence</t>
+  </si>
+  <si>
+    <t>Confidence threshold for Classifier</t>
   </si>
 </sst>
 </file>
@@ -624,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2967,8 +2973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3015,7 +3021,17 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Wait for Completion of Task is working
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -630,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2973,7 +2973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Finished with getting data from ML Skill
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ReQuoteProcess\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\B&amp;W\Updated Docs\New_BW_QAB_Performer_V1-20230215T050827Z-001\BW_QAB_Performer_V1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Static part of logging message. Calling Get Transaction Data.</t>
   </si>
   <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
     <t>OrchestratorQueueFolder</t>
   </si>
   <si>
@@ -237,6 +234,9 @@
   </si>
   <si>
     <t>Confidence threshold for Classifier</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolderPath</t>
   </si>
 </sst>
 </file>
@@ -630,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -681,7 +681,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -689,11 +689,11 @@
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -710,39 +710,39 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
         <v>45</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
         <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
         <v>49</v>
-      </c>
-      <c r="B8" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
         <v>51</v>
-      </c>
-      <c r="B9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -750,7 +750,7 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -758,63 +758,63 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
         <v>59</v>
-      </c>
-      <c r="B14" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19">
         <v>9463</v>
@@ -1869,13 +1869,13 @@
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1948,48 +1948,48 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2973,8 +2973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2993,7 +2993,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -3023,13 +3023,16 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
         <v>69</v>
-      </c>
-      <c r="B2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>